<commit_message>
working on schet factura
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet-faktura.xlsx
+++ b/application/views/rpt/ru/doc/schet-faktura.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Приложение № 1
 к постановлению Правительства
@@ -256,12 +256,6 @@
     <t>{$v-&gt;doc_view-&gt;user_sign}</t>
   </si>
   <si>
-    <t>без акциза</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_code}</t>
-  </si>
-  <si>
     <t>{$v-&gt;rows[]-&gt;vat_rate}</t>
   </si>
   <si>
@@ -272,13 +266,25 @@
   </si>
   <si>
     <t>{$v-&gt;rows[]-&gt;party_label}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_unit_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_accis}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;origin_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;origin_name}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,20 +352,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
@@ -371,6 +363,36 @@
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -390,7 +412,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -779,6 +801,15 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -872,234 +903,270 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="24" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="2" borderId="5" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="31" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="29" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="28" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="9" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="21" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="31" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="29" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="2" borderId="5" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1434,275 +1501,275 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AE25"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="K15" sqref="K15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4" style="1" customWidth="1"/>
-    <col min="4" max="4" width="1.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="1" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="0.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="1.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="0.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="1.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="2.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="0.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="3" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="3.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="1.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="5.85546875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="3.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="2" style="1" customWidth="1"/>
-    <col min="28" max="28" width="2.42578125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="9" style="1" customWidth="1"/>
-    <col min="30" max="30" width="20.28515625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="0.5703125" style="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="1" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="1.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="0.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="0.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="0.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="3" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="3.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="1.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="3.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="2" style="1" customWidth="1"/>
+    <col min="27" max="27" width="2.42578125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="9" style="1" customWidth="1"/>
+    <col min="29" max="29" width="20.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="2.7109375" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:30" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="4" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
     </row>
-    <row r="2" spans="2:31" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+    <row r="2" spans="1:30" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="7"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="2"/>
     </row>
-    <row r="5" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="29" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="2"/>
     </row>
-    <row r="6" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="29" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="29" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="29"/>
-      <c r="T7" s="29"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
-      <c r="AE7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="2"/>
     </row>
-    <row r="8" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
@@ -1723,606 +1790,694 @@
       <c r="AA8" s="29"/>
       <c r="AB8" s="29"/>
       <c r="AC8" s="29"/>
-      <c r="AD8" s="29"/>
-      <c r="AE8" s="7"/>
+      <c r="AD8" s="2"/>
     </row>
-    <row r="9" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="29"/>
-      <c r="X9" s="29"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="29"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="29"/>
-      <c r="AD9" s="29"/>
-      <c r="AE9" s="7"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="2"/>
     </row>
-    <row r="10" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="29"/>
-      <c r="W10" s="29"/>
-      <c r="X10" s="29"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
-      <c r="AB10" s="29"/>
-      <c r="AC10" s="29"/>
-      <c r="AD10" s="29"/>
-      <c r="AE10" s="7"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="2"/>
     </row>
-    <row r="11" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="29"/>
-      <c r="AA11" s="29"/>
-      <c r="AB11" s="29"/>
-      <c r="AC11" s="29"/>
-      <c r="AD11" s="29"/>
-      <c r="AE11" s="7"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="2"/>
     </row>
-    <row r="12" spans="2:31" ht="15.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
+    <row r="12" spans="1:30" ht="15.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="29" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="29"/>
-      <c r="AC12" s="29"/>
-      <c r="AD12" s="29"/>
-      <c r="AE12" s="31"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="28"/>
+      <c r="AD12" s="4"/>
     </row>
-    <row r="13" spans="2:31" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="43" t="s">
+    <row r="13" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="49" t="s">
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="45"/>
-      <c r="N13" s="50" t="s">
+      <c r="L13" s="39"/>
+      <c r="M13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="50" t="s">
+      <c r="N13" s="39"/>
+      <c r="O13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="50" t="s">
+      <c r="P13" s="39"/>
+      <c r="Q13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="S13" s="45"/>
-      <c r="T13" s="50" t="s">
+      <c r="R13" s="39"/>
+      <c r="S13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="U13" s="45"/>
-      <c r="V13" s="51" t="s">
+      <c r="T13" s="39"/>
+      <c r="U13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="W13" s="50" t="s">
+      <c r="V13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="45"/>
-      <c r="Z13" s="46" t="s">
+      <c r="W13" s="38"/>
+      <c r="X13" s="39"/>
+      <c r="Y13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AA13" s="47"/>
-      <c r="AB13" s="47"/>
-      <c r="AC13" s="48"/>
-      <c r="AD13" s="52" t="s">
+      <c r="Z13" s="40"/>
+      <c r="AA13" s="40"/>
+      <c r="AB13" s="41"/>
+      <c r="AC13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AE13" s="53"/>
+      <c r="AD13" s="42"/>
     </row>
-    <row r="14" spans="2:31" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="54"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18" t="s">
+    <row r="14" spans="1:30" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="H14" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="17"/>
-      <c r="Z14" s="12" t="s">
+      <c r="I14" s="46"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="49"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="12" t="s">
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="55"/>
+      <c r="AB14" s="47"/>
+      <c r="AC14" s="44"/>
+      <c r="AD14" s="50"/>
     </row>
-    <row r="15" spans="2:31" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="56" t="s">
+    <row r="15" spans="1:30" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="59" t="s">
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="60" t="s">
+      <c r="H15" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="57"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="61" t="s">
+      <c r="I15" s="52"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="58"/>
-      <c r="N15" s="62" t="s">
+      <c r="L15" s="53"/>
+      <c r="M15" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="58"/>
-      <c r="P15" s="62" t="s">
+      <c r="N15" s="53"/>
+      <c r="O15" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="62" t="s">
+      <c r="P15" s="53"/>
+      <c r="Q15" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="58"/>
-      <c r="T15" s="62" t="s">
+      <c r="R15" s="53"/>
+      <c r="S15" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="U15" s="58"/>
-      <c r="V15" s="59" t="s">
+      <c r="T15" s="53"/>
+      <c r="U15" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="W15" s="62" t="s">
+      <c r="V15" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="X15" s="57"/>
-      <c r="Y15" s="58"/>
-      <c r="Z15" s="62" t="s">
+      <c r="W15" s="52"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="AA15" s="58"/>
-      <c r="AB15" s="62" t="s">
+      <c r="Z15" s="53"/>
+      <c r="AA15" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="AC15" s="58"/>
-      <c r="AD15" s="62" t="s">
+      <c r="AB15" s="53"/>
+      <c r="AC15" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="AE15" s="63"/>
+      <c r="AD15" s="58"/>
     </row>
-    <row r="16" spans="2:31" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="32" t="s">
+    <row r="16" spans="1:30" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35" t="s">
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="64"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="88"/>
+      <c r="M16" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="81"/>
+      <c r="O16" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="R16" s="78"/>
+      <c r="S16" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" s="65"/>
+      <c r="U16" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="V16" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="M16" s="40"/>
-      <c r="N16" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="O16" s="40"/>
-      <c r="P16" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" s="38"/>
-      <c r="T16" s="76" t="s">
-        <v>68</v>
-      </c>
-      <c r="U16" s="38"/>
-      <c r="V16" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="W16" s="39" t="s">
+      <c r="W16" s="80"/>
+      <c r="X16" s="81"/>
+      <c r="Y16" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z16" s="65"/>
+      <c r="AA16" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB16" s="65"/>
+      <c r="AC16" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="40"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="38"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="38"/>
-      <c r="AD16" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE16" s="38"/>
+      <c r="AD16" s="85"/>
     </row>
-    <row r="17" spans="2:31" ht="15.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="65" t="s">
+    <row r="17" spans="1:30" ht="15.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="67" t="s">
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="Q17" s="68"/>
-      <c r="R17" s="69" t="s">
+      <c r="P17" s="70"/>
+      <c r="Q17" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="70"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="71"/>
-      <c r="V17" s="72" t="s">
+      <c r="R17" s="72"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="73"/>
+      <c r="U17" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="W17" s="73" t="s">
+      <c r="V17" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="X17" s="74"/>
-      <c r="Y17" s="75"/>
-      <c r="Z17" s="64"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
-      <c r="AE17" s="21"/>
+      <c r="W17" s="76"/>
+      <c r="X17" s="77"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
     </row>
-    <row r="18" spans="2:31" ht="25.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:31" ht="7.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="22" t="s">
+    <row r="18" spans="1:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:30" ht="7.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="S19" s="22" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="31"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="31"/>
     </row>
-    <row r="20" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="K20" s="23" t="s">
+    <row r="20" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="24"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="30"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="32"/>
     </row>
-    <row r="21" spans="2:31" ht="6.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E21" s="25" t="s">
+    <row r="21" spans="1:30" ht="6.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="K21" s="26" t="s">
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="Y21" s="25" t="s">
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="Z21" s="21"/>
-      <c r="AC21" s="26" t="s">
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31"/>
+      <c r="AB21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="AD21" s="21"/>
+      <c r="AC21" s="34"/>
     </row>
-    <row r="22" spans="2:31" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:31" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="22" t="s">
+    <row r="22" spans="1:30" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
+      <c r="AC22" s="31"/>
+    </row>
+    <row r="23" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="24"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="24"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="32"/>
+      <c r="AA23" s="32"/>
+      <c r="AB23" s="32"/>
+      <c r="AC23" s="32"/>
     </row>
-    <row r="24" spans="2:31" ht="6.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G24" s="25" t="s">
+    <row r="24" spans="1:30" ht="6.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="M24" s="26" t="s">
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="21"/>
-      <c r="S24" s="27" t="s">
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-    </row>
-    <row r="25" spans="2:31" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="37"/>
+      <c r="Z24" s="37"/>
+      <c r="AA24" s="37"/>
+      <c r="AB24" s="37"/>
+      <c r="AC24" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="J3:AD3"/>
-    <mergeCell ref="J4:AD4"/>
-    <mergeCell ref="J5:AD5"/>
-    <mergeCell ref="J6:AD6"/>
-    <mergeCell ref="J7:AD7"/>
-    <mergeCell ref="J8:AD8"/>
-    <mergeCell ref="J9:AD9"/>
-    <mergeCell ref="J10:AD10"/>
-    <mergeCell ref="J11:AD11"/>
-    <mergeCell ref="J12:AD12"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="S19:W20"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="S24:AD25"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="S23:AD23"/>
-    <mergeCell ref="B17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="W17:Y17"/>
-    <mergeCell ref="Z17:AE17"/>
-    <mergeCell ref="AD15:AE15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="T16:U16"/>
-    <mergeCell ref="W16:Y16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AD16:AE16"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="Z15:AA15"/>
-    <mergeCell ref="AB15:AC15"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="B13:G14"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="L13:M14"/>
-    <mergeCell ref="N13:O14"/>
-    <mergeCell ref="P13:Q14"/>
-    <mergeCell ref="R13:S14"/>
-    <mergeCell ref="T13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="W13:Y14"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="AD13:AE14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="C1:T1"/>
-    <mergeCell ref="U1:AE1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="D10:AC10"/>
+    <mergeCell ref="D11:AC11"/>
+    <mergeCell ref="D12:AC12"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="T1:AD1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D3:AC3"/>
+    <mergeCell ref="D4:AC4"/>
+    <mergeCell ref="D5:AC5"/>
+    <mergeCell ref="AC13:AD14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="Q13:R14"/>
+    <mergeCell ref="S13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:X14"/>
+    <mergeCell ref="Y13:AB13"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="A17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:T17"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="Y17:AD17"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="R19:V20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="R24:AC24"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="AB21:AC21"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="L23:O23"/>
+    <mergeCell ref="R23:AC23"/>
+    <mergeCell ref="D6:AC6"/>
+    <mergeCell ref="D7:AC7"/>
+    <mergeCell ref="D8:AC8"/>
+    <mergeCell ref="D9:AC9"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.55118110236220474" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="93" orientation="landscape" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="26" max="16383" man="1"/>
-  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on misell plugin
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet-faktura.xlsx
+++ b/application/views/rpt/ru/doc/schet-faktura.xlsx
@@ -78,206 +78,205 @@
 покупателю</t>
   </si>
   <si>
-    <t>Стоимость то-
-варов (работ,
+    <t>Страна происхож-
+дения товара</t>
+  </si>
+  <si>
+    <t>Номер
+таможенной
+декларации</t>
+  </si>
+  <si>
+    <t>код</t>
+  </si>
+  <si>
+    <t>условное
+обозначе-
+ние(нацио-
+нальное)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">циф-
+ро-
+вой
+код  </t>
+  </si>
+  <si>
+    <t>краткое
+наиме-
+нование</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>2а</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10а</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Всего к оплате</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Х</t>
+  </si>
+  <si>
+    <t>Руководитель организации
+или иное уполномоченное лицо</t>
+  </si>
+  <si>
+    <t>Главный бухгалтер или 
+иное уполномоченное лицо</t>
+  </si>
+  <si>
+    <t>подпись</t>
+  </si>
+  <si>
+    <t>ф.и.о.</t>
+  </si>
+  <si>
+    <t>Индивидуальный предприниматель</t>
+  </si>
+  <si>
+    <t>(реквизиты свидетельства о государственной регистрации индивидуального предпринимателя)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СЧЕТ-ФАКТУРА  №{$v-&gt;doc_view-&gt;view_num} от {$v-&gt;doc_view-&gt;loc_date}
+ИСПРАВЛЕНИЕ  №             от </t>
+  </si>
+  <si>
+    <t>ИНН/КПП продавца:</t>
+  </si>
+  <si>
+    <t>Адрес:</t>
+  </si>
+  <si>
+    <t>Продавец:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Валюта: наименование, код: </t>
+  </si>
+  <si>
+    <t>Российский рубль, 643</t>
+  </si>
+  <si>
+    <t>{$v-&gt;a-&gt;company_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;p-&gt;company_jaddress}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;a-&gt;company_jaddress}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;a-&gt;company_vat_id} / {$v-&gt;a-&gt;company_vat_licence_id}</t>
+  </si>
+  <si>
+    <t>Грузоотправитель и его адрес:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> он же</t>
+  </si>
+  <si>
+    <t>{$v-&gt;p-&gt;company_name}, {$v-&gt;p-&gt;company_jaddress}</t>
+  </si>
+  <si>
+    <t>К платежно-расчетному документу:</t>
+  </si>
+  <si>
+    <t>{$v-&gt;p-&gt;company_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;p-&gt;company_vat_id} / {$v-&gt;p-&gt;company_vat_licence_id}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_unit}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_quantity}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_price}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_sum}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{$v-&gt;footer-&gt;vat} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {$v-&gt;footer-&gt;total}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;doc_view-&gt;user_sign}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;vat_rate}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_sum_total}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_sum_vat}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;party_label}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_unit_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_accis}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;origin_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;origin_name}</t>
+  </si>
+  <si>
+    <t>Стоимость товаров (работ,
 услуг), иму-
 щественных
 прав с на-
 логом - всего</t>
-  </si>
-  <si>
-    <t>Страна происхож-
-дения товара</t>
-  </si>
-  <si>
-    <t>Номер
-таможенной
-декларации</t>
-  </si>
-  <si>
-    <t>код</t>
-  </si>
-  <si>
-    <t>условное
-обозначе-
-ние(нацио-
-нальное)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">циф-
-ро-
-вой
-код  </t>
-  </si>
-  <si>
-    <t>краткое
-наиме-
-нование</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2а</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>10а</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Всего к оплате</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Х</t>
-  </si>
-  <si>
-    <t>Руководитель организации
-или иное уполномоченное лицо</t>
-  </si>
-  <si>
-    <t>Главный бухгалтер или 
-иное уполномоченное лицо</t>
-  </si>
-  <si>
-    <t>подпись</t>
-  </si>
-  <si>
-    <t>ф.и.о.</t>
-  </si>
-  <si>
-    <t>Индивидуальный предприниматель</t>
-  </si>
-  <si>
-    <t>(реквизиты свидетельства о государственной регистрации индивидуального предпринимателя)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СЧЕТ-ФАКТУРА  №{$v-&gt;doc_view-&gt;view_num} от {$v-&gt;doc_view-&gt;loc_date}
-ИСПРАВЛЕНИЕ  №             от </t>
-  </si>
-  <si>
-    <t>ИНН/КПП продавца:</t>
-  </si>
-  <si>
-    <t>Адрес:</t>
-  </si>
-  <si>
-    <t>Продавец:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Валюта: наименование, код: </t>
-  </si>
-  <si>
-    <t>Российский рубль, 643</t>
-  </si>
-  <si>
-    <t>{$v-&gt;a-&gt;company_name}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;p-&gt;company_jaddress}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;a-&gt;company_jaddress}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;a-&gt;company_vat_id} / {$v-&gt;a-&gt;company_vat_licence_id}</t>
-  </si>
-  <si>
-    <t>Грузоотправитель и его адрес:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> он же</t>
-  </si>
-  <si>
-    <t>{$v-&gt;p-&gt;company_name}, {$v-&gt;p-&gt;company_jaddress}</t>
-  </si>
-  <si>
-    <t>К платежно-расчетному документу:</t>
-  </si>
-  <si>
-    <t>{$v-&gt;p-&gt;company_name}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;p-&gt;company_vat_id} / {$v-&gt;p-&gt;company_vat_licence_id}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_name}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_unit}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_quantity}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_price}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_sum}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{$v-&gt;footer-&gt;vat} </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {$v-&gt;footer-&gt;total}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;doc_view-&gt;user_sign}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;vat_rate}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_sum_total}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_sum_vat}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;party_label}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_unit_code}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;product_accis}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;origin_code}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;rows[]-&gt;origin_name}</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1503,7 @@
   <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:L15"/>
+      <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1544,7 +1543,7 @@
   <sheetData>
     <row r="1" spans="1:30" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1580,12 +1579,12 @@
     <row r="2" spans="1:30" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1616,12 +1615,12 @@
     </row>
     <row r="4" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1652,12 +1651,12 @@
     </row>
     <row r="5" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
       <c r="D5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -1688,12 +1687,12 @@
     </row>
     <row r="6" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1729,7 +1728,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1760,7 +1759,7 @@
     </row>
     <row r="8" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1799,7 +1798,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1835,7 +1834,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1871,7 +1870,7 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1902,12 +1901,12 @@
     </row>
     <row r="12" spans="1:30" ht="15.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="28"/>
@@ -1975,18 +1974,18 @@
         <v>12</v>
       </c>
       <c r="V13" s="16" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="W13" s="38"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z13" s="40"/>
       <c r="AA13" s="40"/>
       <c r="AB13" s="41"/>
       <c r="AC13" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AD13" s="42"/>
     </row>
@@ -1998,10 +1997,10 @@
       <c r="E14" s="44"/>
       <c r="F14" s="45"/>
       <c r="G14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="I14" s="46"/>
       <c r="J14" s="47"/>
@@ -2020,11 +2019,11 @@
       <c r="W14" s="44"/>
       <c r="X14" s="45"/>
       <c r="Y14" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Z14" s="47"/>
       <c r="AA14" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AB14" s="47"/>
       <c r="AC14" s="44"/>
@@ -2032,7 +2031,7 @@
     </row>
     <row r="15" spans="1:30" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="83"/>
       <c r="C15" s="83"/>
@@ -2040,57 +2039,57 @@
       <c r="E15" s="83"/>
       <c r="F15" s="84"/>
       <c r="G15" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="55" t="s">
         <v>21</v>
-      </c>
-      <c r="H15" s="55" t="s">
-        <v>22</v>
       </c>
       <c r="I15" s="52"/>
       <c r="J15" s="53"/>
       <c r="K15" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L15" s="53"/>
       <c r="M15" s="57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N15" s="53"/>
       <c r="O15" s="57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P15" s="53"/>
       <c r="Q15" s="57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R15" s="53"/>
       <c r="S15" s="57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T15" s="53"/>
       <c r="U15" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="V15" s="57" t="s">
         <v>28</v>
-      </c>
-      <c r="V15" s="57" t="s">
-        <v>29</v>
       </c>
       <c r="W15" s="52"/>
       <c r="X15" s="53"/>
       <c r="Y15" s="57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Z15" s="53"/>
       <c r="AA15" s="57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB15" s="53"/>
       <c r="AC15" s="57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AD15" s="58"/>
     </row>
     <row r="16" spans="1:30" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="60"/>
       <c r="C16" s="60"/>
@@ -2098,57 +2097,57 @@
       <c r="E16" s="60"/>
       <c r="F16" s="61"/>
       <c r="G16" s="62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I16" s="64"/>
       <c r="J16" s="65"/>
       <c r="K16" s="87" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L16" s="88"/>
       <c r="M16" s="79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N16" s="81"/>
       <c r="O16" s="79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P16" s="81"/>
       <c r="Q16" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R16" s="78"/>
       <c r="S16" s="66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T16" s="65"/>
       <c r="U16" s="82" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V16" s="79" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W16" s="80"/>
       <c r="X16" s="81"/>
       <c r="Y16" s="63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Z16" s="65"/>
       <c r="AA16" s="63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB16" s="65"/>
       <c r="AC16" s="85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AD16" s="85"/>
     </row>
     <row r="17" spans="1:30" ht="15.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="68"/>
       <c r="C17" s="68"/>
@@ -2164,20 +2163,20 @@
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
       <c r="O17" s="69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P17" s="70"/>
       <c r="Q17" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R17" s="72"/>
       <c r="S17" s="72"/>
       <c r="T17" s="73"/>
       <c r="U17" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="V17" s="75" t="s">
         <v>63</v>
-      </c>
-      <c r="V17" s="75" t="s">
-        <v>64</v>
       </c>
       <c r="W17" s="76"/>
       <c r="X17" s="77"/>
@@ -2191,7 +2190,7 @@
     <row r="18" spans="1:30" ht="25.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:30" ht="7.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="31"/>
@@ -2210,7 +2209,7 @@
       <c r="P19" s="31"/>
       <c r="Q19" s="31"/>
       <c r="R19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S19" s="30"/>
       <c r="T19" s="30"/>
@@ -2235,7 +2234,7 @@
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
       <c r="J20" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K20" s="32"/>
       <c r="L20" s="32"/>
@@ -2262,7 +2261,7 @@
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
       <c r="D21" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="34"/>
       <c r="F21" s="34"/>
@@ -2270,7 +2269,7 @@
       <c r="H21" s="34"/>
       <c r="I21" s="31"/>
       <c r="J21" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
@@ -2286,13 +2285,13 @@
       <c r="V21" s="31"/>
       <c r="W21" s="31"/>
       <c r="X21" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y21" s="34"/>
       <c r="Z21" s="31"/>
       <c r="AA21" s="31"/>
       <c r="AB21" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC21" s="34"/>
     </row>
@@ -2329,7 +2328,7 @@
     </row>
     <row r="23" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
@@ -2367,7 +2366,7 @@
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
       <c r="F24" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
@@ -2375,7 +2374,7 @@
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
       <c r="L24" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
@@ -2383,7 +2382,7 @@
       <c r="P24" s="31"/>
       <c r="Q24" s="31"/>
       <c r="R24" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S24" s="37"/>
       <c r="T24" s="37"/>

</xml_diff>

<commit_message>
schet factura upd fixed
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet-faktura.xlsx
+++ b/application/views/rpt/ru/doc/schet-faktura.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">ИНН/КПП покупателя</t>
   </si>
   <si>
-    <t xml:space="preserve">{$v-&gt;buyer-&gt;company_tax_id} / {$v-&gt;buyer-&gt;company_tax_id}</t>
+    <t xml:space="preserve">{$v-&gt;buyer-&gt;company_tax_id} / {$v-&gt;buyer-&gt;company_tax_id2}</t>
   </si>
   <si>
     <t xml:space="preserve">Валюта: наименование, код</t>
@@ -606,18 +606,18 @@
   <dimension ref="A1:AK32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP8" activeCellId="0" sqref="AP8"/>
+      <selection pane="topLeft" activeCell="AK13" activeCellId="0" sqref="AK13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="1.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="2.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="1.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="1.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="2.7"/>
@@ -625,16 +625,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="2.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="1.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="1.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="3.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="1.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="1.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="1.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="4.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="3.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="17.76"/>
   </cols>

</xml_diff>

<commit_message>
schet factura schet factura fixed
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/schet-faktura.xlsx
+++ b/application/views/rpt/ru/doc/schet-faktura.xlsx
@@ -226,7 +226,7 @@
     <t xml:space="preserve">{$v-&gt;rows[]-&gt;product_name}</t>
   </si>
   <si>
-    <t xml:space="preserve">{$v-&gt;rows[]-&gt;product_code}</t>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">{$v-&gt;rows[]-&gt;product_unit_code}</t>
@@ -606,10 +606,10 @@
   <dimension ref="A1:AK32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK13" activeCellId="0" sqref="AK13"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.38"/>
@@ -617,7 +617,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="1.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="2.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="1.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="1.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="2.7"/>

</xml_diff>